<commit_message>
Changed precision crossing mode to parameters that can be set in the test case file.
</commit_message>
<xml_diff>
--- a/BackTestingResults/Statistics.xlsx
+++ b/BackTestingResults/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Symbol</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Taker Fee %</t>
   </si>
   <si>
+    <t>Precision Crossing</t>
+  </si>
+  <si>
     <t>Wins</t>
   </si>
   <si>
@@ -79,7 +82,7 @@
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>2021-06-01</t>
+    <t>2021-07-01</t>
   </si>
   <si>
     <t>2021-12-01</t>
@@ -88,7 +91,10 @@
     <t>30</t>
   </si>
   <si>
-    <t>48.0%</t>
+    <t>49.4%</t>
+  </si>
+  <si>
+    <t>48.8%</t>
   </si>
 </sst>
 </file>
@@ -446,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -513,22 +519,25 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>10000</v>
@@ -545,35 +554,103 @@
       <c r="J2">
         <v>0.075</v>
       </c>
-      <c r="K2">
-        <v>49</v>
+      <c r="K2" t="b">
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="M2">
-        <v>102</v>
-      </c>
-      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2">
+        <v>87</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2">
+        <v>-6</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>6450</v>
+      </c>
+      <c r="S2">
+        <v>-4400</v>
+      </c>
+      <c r="T2">
+        <v>875.7125000000002</v>
+      </c>
+      <c r="U2">
+        <v>1174.2875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="O2">
-        <v>-7</v>
-      </c>
-      <c r="P2">
-        <v>5</v>
-      </c>
-      <c r="Q2">
-        <v>7350</v>
-      </c>
-      <c r="R2">
-        <v>-5300</v>
-      </c>
-      <c r="S2">
-        <v>1040.8625</v>
-      </c>
-      <c r="T2">
-        <v>1009.1375</v>
+      <c r="F3">
+        <v>10000</v>
+      </c>
+      <c r="G3">
+        <v>1.5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>-0.025</v>
+      </c>
+      <c r="J3">
+        <v>0.075</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>41</v>
+      </c>
+      <c r="M3">
+        <v>43</v>
+      </c>
+      <c r="N3">
+        <v>84</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3">
+        <v>-5</v>
+      </c>
+      <c r="Q3">
+        <v>7</v>
+      </c>
+      <c r="R3">
+        <v>6150</v>
+      </c>
+      <c r="S3">
+        <v>-4300</v>
+      </c>
+      <c r="T3">
+        <v>850.7125000000003</v>
+      </c>
+      <c r="U3">
+        <v>999.2874999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed int/float bug when reading data from ByBit in find_crossing() function.
</commit_message>
<xml_diff>
--- a/BackTestingResults/Statistics.xlsx
+++ b/BackTestingResults/Statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Symbol</t>
   </si>
@@ -79,10 +79,10 @@
     <t>Test #</t>
   </si>
   <si>
-    <t>BTCUSDT</t>
-  </si>
-  <si>
-    <t>2021-07-01</t>
+    <t>BTCUSD</t>
+  </si>
+  <si>
+    <t>2021-11-01</t>
   </si>
   <si>
     <t>2021-12-01</t>
@@ -91,10 +91,7 @@
     <t>30</t>
   </si>
   <si>
-    <t>49.4%</t>
-  </si>
-  <si>
-    <t>48.8%</t>
+    <t>26.7%</t>
   </si>
 </sst>
 </file>
@@ -452,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,7 +522,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -543,10 +540,10 @@
         <v>10000</v>
       </c>
       <c r="G2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I2">
         <v>-0.025</v>
@@ -555,102 +552,37 @@
         <v>0.075</v>
       </c>
       <c r="K2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="M2">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="N2">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
       </c>
       <c r="P2">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>6450</v>
+        <v>400</v>
       </c>
       <c r="S2">
-        <v>-4400</v>
+        <v>-733.333333333333</v>
       </c>
       <c r="T2">
-        <v>875.7125000000002</v>
+        <v>185</v>
       </c>
       <c r="U2">
-        <v>1174.2875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <v>10000</v>
-      </c>
-      <c r="G3">
-        <v>1.5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>-0.025</v>
-      </c>
-      <c r="J3">
-        <v>0.075</v>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>41</v>
-      </c>
-      <c r="M3">
-        <v>43</v>
-      </c>
-      <c r="N3">
-        <v>84</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3">
-        <v>-5</v>
-      </c>
-      <c r="Q3">
-        <v>7</v>
-      </c>
-      <c r="R3">
-        <v>6150</v>
-      </c>
-      <c r="S3">
-        <v>-4300</v>
-      </c>
-      <c r="T3">
-        <v>850.7125000000003</v>
-      </c>
-      <c r="U3">
-        <v>999.2874999999997</v>
+        <v>-518.333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created main.py file to be able to run the application outside JupyterLab.
</commit_message>
<xml_diff>
--- a/BackTestingResults/Statistics.xlsx
+++ b/BackTestingResults/Statistics.xlsx
@@ -1,123 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Interval</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>TP %</t>
-  </si>
-  <si>
-    <t>SL %</t>
-  </si>
-  <si>
-    <t>Maker Fee %</t>
-  </si>
-  <si>
-    <t>Taker Fee %</t>
-  </si>
-  <si>
-    <t>Precision Crossing</t>
-  </si>
-  <si>
-    <t>Wins</t>
-  </si>
-  <si>
-    <t>Losses</t>
-  </si>
-  <si>
-    <t>Total Trades</t>
-  </si>
-  <si>
-    <t>Success Rate</t>
-  </si>
-  <si>
-    <t>Loss Idx</t>
-  </si>
-  <si>
-    <t>Win Idx</t>
-  </si>
-  <si>
-    <t>Wins $</t>
-  </si>
-  <si>
-    <t>Losses $</t>
-  </si>
-  <si>
-    <t>Fees $</t>
-  </si>
-  <si>
-    <t>Total P/L</t>
-  </si>
-  <si>
-    <t>Test #</t>
-  </si>
-  <si>
-    <t>BTCUSD</t>
-  </si>
-  <si>
-    <t>2021-11-01</t>
-  </si>
-  <si>
-    <t>2021-12-01</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>26.7%</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -132,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -448,144 +420,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Test #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Interval</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TP %</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SL %</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Maker Fee %</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Taker Fee %</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Precision Crossing</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Losses</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Total Trades</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Success Rate</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Loss Idx</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Win Idx</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Wins $</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Losses $</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Fees $</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Total P/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2021-11-01</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2021-12-01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2">
-        <v>10000</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>-0.025</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="n">
         <v>0.075</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="n">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="n">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2">
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>26.7%</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
         <v>-10</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
-      <c r="R2">
+      <c r="R2" t="n">
         <v>400</v>
       </c>
-      <c r="S2">
+      <c r="S2" t="n">
         <v>-733.333333333333</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="n">
         <v>185</v>
       </c>
-      <c r="U2">
+      <c r="U2" t="n">
         <v>-518.333333333333</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>